<commit_message>
Updated geometry to reflect current radiator selection
</commit_message>
<xml_diff>
--- a/Output/Sizing Results.xlsx
+++ b/Output/Sizing Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbsei\Documents\MATLAB\AEROSP 583\Thermal Code\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5DBC4B-0405-449D-B687-BEAD4E1D6FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08777129-C016-468D-8CD2-5FCF5CDBEEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11250" yWindow="0" windowWidth="11250" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hot Case" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
-  <si>
-    <t>AZJ-4020</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -124,6 +121,9 @@
   </si>
   <si>
     <t>Eps eta:</t>
+  </si>
+  <si>
+    <t>AZ-93</t>
   </si>
 </sst>
 </file>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:R6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -508,7 +508,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -516,10 +516,10 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -531,83 +531,83 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="R2" s="4"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>0.14499999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="F3">
-        <v>0.88</v>
+        <v>0.91</v>
       </c>
       <c r="G3">
         <f>SUM(H3:Q3)</f>
-        <v>1.4448999999999999</v>
+        <v>1.3934</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -628,10 +628,10 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1.0999999999999999E-2</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="O3">
-        <v>1.4339</v>
+        <v>1.3927</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -645,16 +645,16 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>0.09</v>
@@ -702,16 +702,16 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>0.28000000000000003</v>
@@ -759,13 +759,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="9">
         <f>0.74/0.91</f>
@@ -786,27 +786,27 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>0.14499999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="F7" s="1">
         <f>$F$6*F3</f>
-        <v>0.71560439560439559</v>
+        <v>0.74</v>
       </c>
       <c r="G7">
         <f>SUM(H7:Q7)</f>
-        <v>1.8276000000000001</v>
+        <v>1.774</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -827,10 +827,10 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>1.38E-2</v>
+        <v>8.0100000000000005E-2</v>
       </c>
       <c r="O7">
-        <v>1.8138000000000001</v>
+        <v>1.6939</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>0.09</v>
@@ -902,16 +902,16 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>0.28000000000000003</v>
@@ -968,15 +968,16 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3AED50-2B12-435B-866B-1ECAC22D1C0D}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:R4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -988,13 +989,13 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -1006,95 +1007,67 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="R2" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="9">
-        <f>0.74/0.91</f>
-        <v>0.81318681318681318</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:F1"/>
+  <mergeCells count="4">
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:Q1"/>
     <mergeCell ref="R1:R2"/>
-    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated sizing results excel doc
</commit_message>
<xml_diff>
--- a/Output/Sizing Results.xlsx
+++ b/Output/Sizing Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbsei\Documents\MATLAB\AEROSP 583\Thermal Code\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08777129-C016-468D-8CD2-5FCF5CDBEEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BDCFD6-6F78-424F-9EB7-DB7E8FA9BF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11250" yWindow="0" windowWidth="11250" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11250" yWindow="0" windowWidth="11250" windowHeight="14400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hot Case" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -124,6 +124,27 @@
   </si>
   <si>
     <t>AZ-93</t>
+  </si>
+  <si>
+    <t>NASA GSFC</t>
+  </si>
+  <si>
+    <t>Temp Min [C]</t>
+  </si>
+  <si>
+    <t>Temp Max [C]</t>
+  </si>
+  <si>
+    <t>Dark Mirror SiO-Cr-Al</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Teflon Impregnated Anodized Titanium</t>
+  </si>
+  <si>
+    <t>SiOx/VDA/0.5mil Kapton</t>
   </si>
 </sst>
 </file>
@@ -192,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -213,6 +234,7 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -974,13 +996,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3AED50-2B12-435B-866B-1ECAC22D1C0D}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.9296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
@@ -989,8 +1017,12 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
+      <c r="E1" s="8">
+        <v>0.13</v>
+      </c>
+      <c r="F1" s="9">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
@@ -1018,10 +1050,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>7</v>
@@ -1061,6 +1093,48 @@
         <v>21</v>
       </c>
       <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3">
+        <v>0.86</v>
+      </c>
+      <c r="F3">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>0.19</v>
+      </c>
+      <c r="F4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <v>0.76</v>
+      </c>
+      <c r="F5">
+        <v>0.26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>